<commit_message>
update json_parser and json_reader
</commit_message>
<xml_diff>
--- a/doc/MessageDesign.xlsx
+++ b/doc/MessageDesign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13650" tabRatio="647" firstSheet="6" activeTab="9"/>
+    <workbookView windowWidth="21495" windowHeight="10545" tabRatio="647" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="MessageId" sheetId="1" r:id="rId1"/>
@@ -2832,7 +2832,7 @@
   <dimension ref="A1:AN20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>

</xml_diff>